<commit_message>
2018-06-08 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7CCA8A-BBE1-45CC-9251-D842C36B578F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A90D963-6D47-4207-B05F-F35F949FDE87}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="4" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>h8o4</t>
+  </si>
+  <si>
+    <t>10o57RT</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F26E1D-C787-4768-8B4F-FA812045F04F}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1780,7 +1783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F47D43-073E-45FD-86E6-4FD8DA735988}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1923,7 +1926,9 @@
       <c r="G10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>

</xml_diff>

<commit_message>
2018-06-10 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6E271D-4FB6-47D7-801A-1499382E15F6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FCE62A-6E58-483E-B3AB-D7B0E91D05D1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>10o64</t>
+  </si>
+  <si>
+    <t>h7r59</t>
+  </si>
+  <si>
+    <t>13o70</t>
+  </si>
+  <si>
+    <t>12b52</t>
+  </si>
+  <si>
+    <t>12w52SO</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1804,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1940,16 +1952,24 @@
       <c r="I10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>

</xml_diff>

<commit_message>
2018-06-14 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEC6DB6-33F7-44C5-A8D2-968640207B27}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F510E0F-417F-4AD9-9775-256BDC3A0F61}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -291,6 +291,21 @@
   </si>
   <si>
     <t>2r15</t>
+  </si>
+  <si>
+    <t>5w11</t>
+  </si>
+  <si>
+    <t>4w72</t>
+  </si>
+  <si>
+    <t>13r12</t>
+  </si>
+  <si>
+    <t>12w61</t>
+  </si>
+  <si>
+    <t>11o9</t>
   </si>
 </sst>
 </file>
@@ -405,16 +420,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1008,19 +1023,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1297,19 +1312,19 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1559,19 +1574,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1839,19 +1854,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1867,7 +1882,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1950,10 +1965,10 @@
       <c r="J8" s="3">
         <v>8</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="6">
         <v>9</v>
       </c>
-      <c r="L8" s="9"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
@@ -1983,10 +1998,10 @@
       <c r="J9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="9"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
@@ -2016,10 +2031,10 @@
       <c r="J10" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="8" t="s">
+      <c r="K10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="9"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
@@ -2049,10 +2064,10 @@
       <c r="J11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="9"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
@@ -2067,13 +2082,23 @@
       <c r="E12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="9"/>
+      <c r="F12" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
@@ -2087,8 +2112,8 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="9"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
@@ -2102,8 +2127,8 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="9"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
@@ -2117,8 +2142,8 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="9"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
@@ -2132,8 +2157,8 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="9"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
@@ -2147,8 +2172,8 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -2162,23 +2187,23 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
2018-06-17 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylielennon\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7561C64-9F75-4605-8EFC-E8C9FD7847D6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB1342A-B1C8-4351-AD75-4C746C0C3C96}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="4" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>h10b6</t>
+  </si>
+  <si>
+    <t>11o23</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F26E1D-C787-4768-8B4F-FA812045F04F}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -1904,7 +1907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F47D43-073E-45FD-86E6-4FD8DA735988}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2144,7 +2147,9 @@
       <c r="G13" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="6"/>

</xml_diff>

<commit_message>
2018-06-21 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388C80D0-96A1-4DF7-8521-24F4E934BDFD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC4ED13-FDD6-48CF-8F8D-90C7CF8006FF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="4" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>d8c12</t>
+  </si>
+  <si>
+    <t>10o7</t>
   </si>
 </sst>
 </file>
@@ -1649,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F26E1D-C787-4768-8B4F-FA812045F04F}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1935,7 +1938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F47D43-073E-45FD-86E6-4FD8DA735988}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -2202,7 +2205,9 @@
       <c r="E14" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>

</xml_diff>

<commit_message>
2018-06-24 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylielennon\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1513099-D734-41E1-82F2-4C69A9CF165C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA48124-ED63-4031-AFC1-8BB30C51ED1D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="4" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -336,6 +336,18 @@
   </si>
   <si>
     <t>d8C12</t>
+  </si>
+  <si>
+    <t>2r18</t>
+  </si>
+  <si>
+    <t>h3w19</t>
+  </si>
+  <si>
+    <t>19F11</t>
+  </si>
+  <si>
+    <t>12b29</t>
   </si>
 </sst>
 </file>
@@ -1631,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F26E1D-C787-4768-8B4F-FA812045F04F}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1917,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F47D43-073E-45FD-86E6-4FD8DA735988}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2160,16 +2172,24 @@
       <c r="H13" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="6"/>
+      <c r="I13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>

</xml_diff>

<commit_message>
2018-06-28 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025AEEB0-FEA7-40AA-9AC0-03E7A6CB74E5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B70D25-67D0-4DB2-A8E0-B0C8B929D421}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="5" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
   <si>
     <t>Date</t>
   </si>
@@ -405,6 +405,12 @@
   </si>
   <si>
     <t>3w56</t>
+  </si>
+  <si>
+    <t>h3w10</t>
+  </si>
+  <si>
+    <t>h2b33</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +1995,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2315,8 +2321,12 @@
       <c r="C16" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>

</xml_diff>

<commit_message>
2018-07-10 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B32B1A2-8BAF-4752-8465-3AA7E459E61F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E48F6E4-6E85-4887-B2E2-92E013D0DFD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="154">
   <si>
     <t>Date</t>
   </si>
@@ -481,6 +481,18 @@
   </si>
   <si>
     <t>h1A5</t>
+  </si>
+  <si>
+    <t>10w40</t>
+  </si>
+  <si>
+    <t>14b52</t>
+  </si>
+  <si>
+    <t>10o4</t>
+  </si>
+  <si>
+    <t>11w11</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2491,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2586,10 +2598,18 @@
       <c r="G9" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="6"/>
+      <c r="H9" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
2018-07-12 free run check
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E48F6E4-6E85-4887-B2E2-92E013D0DFD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEF3BB9-FDFF-475E-9C3E-15215525EFB8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="155">
   <si>
     <t>Date</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>11w11</t>
+  </si>
+  <si>
+    <t>18w25</t>
   </si>
 </sst>
 </file>
@@ -2491,7 +2494,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2616,7 +2619,9 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>

<commit_message>
2018-07-15 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E59B0A3-D127-4442-B6BA-1A13C9748BAE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDDC0DE-BC05-4174-A483-95DB9D15661F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="165">
   <si>
     <t>Date</t>
   </si>
@@ -520,6 +520,12 @@
   </si>
   <si>
     <t>h1B5</t>
+  </si>
+  <si>
+    <t>10w68</t>
+  </si>
+  <si>
+    <t>3w18</t>
   </si>
 </sst>
 </file>
@@ -2518,7 +2524,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2676,8 +2682,12 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>

</xml_diff>

<commit_message>
2018-07-17 free run update
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7ABDC7-B25B-425C-8D31-C4543E6211EF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CD36AB-CBC1-41AE-8D80-283792AE1B1E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="167">
   <si>
     <t>Date</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t>h7r60</t>
+  </si>
+  <si>
+    <t>h3o18</t>
   </si>
 </sst>
 </file>
@@ -2527,7 +2530,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2694,7 +2697,9 @@
       <c r="E11" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>166</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>

</xml_diff>

<commit_message>
free run update 2018-07-26
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81EFE48-434D-420A-A472-7025D7FF24AE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCE8293-3777-4FCF-BA22-20EF51782B81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="178">
   <si>
     <t>Date</t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t>4o75</t>
+  </si>
+  <si>
+    <t>h2b23</t>
   </si>
 </sst>
 </file>
@@ -2560,7 +2563,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2766,7 +2769,9 @@
       <c r="G12" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>177</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="6"/>

</xml_diff>

<commit_message>
2018-07-29 free run check
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15706002-0CD5-424E-96E9-AFEF4C7FB823}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05529AD-5816-4AB0-A165-14CB045262AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="183">
   <si>
     <t>Date</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>h2b8</t>
+  </si>
+  <si>
+    <t>h6w29</t>
+  </si>
+  <si>
+    <t>11o60</t>
+  </si>
+  <si>
+    <t>ho11B2</t>
   </si>
 </sst>
 </file>
@@ -2569,7 +2578,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2784,15 +2793,21 @@
       <c r="J12" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="K12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>

</xml_diff>

<commit_message>
2018-07-31 free run upd
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05529AD-5816-4AB0-A165-14CB045262AF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7904DEE-BCCC-4BB8-95F1-EB424F0E2546}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="6" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="187">
   <si>
     <t>Date</t>
   </si>
@@ -580,6 +580,18 @@
   </si>
   <si>
     <t>ho11B2</t>
+  </si>
+  <si>
+    <t>h9w1</t>
+  </si>
+  <si>
+    <t>h5r3</t>
+  </si>
+  <si>
+    <t>10w13</t>
+  </si>
+  <si>
+    <t>13o9</t>
   </si>
 </sst>
 </file>
@@ -2578,7 +2590,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2808,10 +2820,18 @@
       <c r="D13" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="6"/>

</xml_diff>

<commit_message>
randomizing and data entry
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358D202-5AF5-4B2D-9774-2B2855DE560C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5A0EB2-0DFA-43F5-BC7F-DC445F763A2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" activeTab="11" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="491">
   <si>
     <t>Date</t>
   </si>
@@ -1277,15 +1277,9 @@
     <t>2018-09-12 started</t>
   </si>
   <si>
-    <t>Genetic control for apple race, 2018 collection year, day 13(2018-08-28)</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
-    <t>nb#004, page 162,158</t>
-  </si>
-  <si>
     <t>A13-1</t>
   </si>
   <si>
@@ -1376,7 +1370,145 @@
     <t>A13-30</t>
   </si>
   <si>
-    <t>tubes for cohortday 12 genetic control; fill in later</t>
+    <t>A14-1</t>
+  </si>
+  <si>
+    <t>A14-2</t>
+  </si>
+  <si>
+    <t>A14-3</t>
+  </si>
+  <si>
+    <t>A14-4</t>
+  </si>
+  <si>
+    <t>A14-5</t>
+  </si>
+  <si>
+    <t>A14-6</t>
+  </si>
+  <si>
+    <t>A14-7</t>
+  </si>
+  <si>
+    <t>A14-8</t>
+  </si>
+  <si>
+    <t>A14-9</t>
+  </si>
+  <si>
+    <t>A14-10</t>
+  </si>
+  <si>
+    <t>A14-11</t>
+  </si>
+  <si>
+    <t>A14-12</t>
+  </si>
+  <si>
+    <t>A14-13</t>
+  </si>
+  <si>
+    <t>A14-14</t>
+  </si>
+  <si>
+    <t>A14-15</t>
+  </si>
+  <si>
+    <t>A14-16</t>
+  </si>
+  <si>
+    <t>A14-17</t>
+  </si>
+  <si>
+    <t>A14-18</t>
+  </si>
+  <si>
+    <t>A14-19</t>
+  </si>
+  <si>
+    <t>A14-20</t>
+  </si>
+  <si>
+    <t>A14-21</t>
+  </si>
+  <si>
+    <t>A14-22</t>
+  </si>
+  <si>
+    <t>A14-23</t>
+  </si>
+  <si>
+    <t>A14-24</t>
+  </si>
+  <si>
+    <t>A14-25</t>
+  </si>
+  <si>
+    <t>A14-26</t>
+  </si>
+  <si>
+    <t>A14-27</t>
+  </si>
+  <si>
+    <t>A14-28</t>
+  </si>
+  <si>
+    <t>A14-29</t>
+  </si>
+  <si>
+    <t>A14-30</t>
+  </si>
+  <si>
+    <t>nb#004, page 162,158, 164</t>
+  </si>
+  <si>
+    <t>Genetic control for apple race, 2018 collection year, day 13(2018-08-28); Genetic control for apple race, 2018 collection year, day 14(2018-08-29) ;cohort day 12 (2018-08-27) day 15 treatment (2018-09-11) genetic control</t>
+  </si>
+  <si>
+    <t>a12r3_18</t>
+  </si>
+  <si>
+    <t>a12r6_18</t>
+  </si>
+  <si>
+    <t>a12r7_18</t>
+  </si>
+  <si>
+    <t>a12r11_18</t>
+  </si>
+  <si>
+    <t>a12r15_18</t>
+  </si>
+  <si>
+    <t>a12r17_18</t>
+  </si>
+  <si>
+    <t>a12r19_18</t>
+  </si>
+  <si>
+    <t>a12r20_18</t>
+  </si>
+  <si>
+    <t>a12o1_18</t>
+  </si>
+  <si>
+    <t>a12o2_18</t>
+  </si>
+  <si>
+    <t>a12o4_18</t>
+  </si>
+  <si>
+    <t>a12o8_18</t>
+  </si>
+  <si>
+    <t>a12o9_18</t>
+  </si>
+  <si>
+    <t>a12o14_18</t>
+  </si>
+  <si>
+    <t>a12o16_18</t>
   </si>
 </sst>
 </file>
@@ -1503,13 +1635,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2239,19 +2371,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2632,19 +2764,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2658,11 +2790,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61BF6A5-3FBD-4D1E-A656-FF29C6F41ED4}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="15.375" style="2"/>
@@ -2681,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>413</v>
+        <v>475</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -2697,20 +2829,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>415</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2751,32 +2886,66 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="C9" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>477</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>484</v>
+      </c>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="C10" s="8" t="s">
+        <v>485</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>490</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>416</v>
+      </c>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2784,31 +2953,31 @@
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="L11" s="3"/>
     </row>
@@ -2817,31 +2986,31 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L12" s="3"/>
     </row>
@@ -2850,31 +3019,31 @@
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L13" s="3"/>
     </row>
@@ -2883,59 +3052,113 @@
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+        <v>446</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>452</v>
+      </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>461</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>470</v>
+      </c>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>473</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2960,19 +3183,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3213,19 +3436,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3514,19 +3737,19 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3776,19 +3999,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4064,19 +4287,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4478,19 +4701,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4872,19 +5095,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5262,19 +5485,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
entering sotrage data for tomorrow's resp
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED42F3F-B88C-4320-81C2-C4B9899A8C53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16F8447-64A2-44D7-A7A9-37D64B28FC9A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="1" activeTab="13" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="649">
   <si>
     <t>Date</t>
   </si>
@@ -1858,9 +1858,6 @@
     <t>A-2-7-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Genetic control samples; cohorts 7+22 (2018-09-06); </t>
-  </si>
-  <si>
     <t>A-2-8-12</t>
   </si>
   <si>
@@ -1910,6 +1907,84 @@
   </si>
   <si>
     <t>4 cohorts , color coded on the spreadsheet</t>
+  </si>
+  <si>
+    <t>a9_b3_18</t>
+  </si>
+  <si>
+    <t>a24_b4_18</t>
+  </si>
+  <si>
+    <t>a9_b12_18</t>
+  </si>
+  <si>
+    <t>a9_b5_18</t>
+  </si>
+  <si>
+    <t>a9_b13_18</t>
+  </si>
+  <si>
+    <t>a9_b15_18</t>
+  </si>
+  <si>
+    <t>a9_b17_18</t>
+  </si>
+  <si>
+    <t>a9_b23_18</t>
+  </si>
+  <si>
+    <t>a9_b24_18</t>
+  </si>
+  <si>
+    <t>a9_b34_18</t>
+  </si>
+  <si>
+    <t>a24_b35_18</t>
+  </si>
+  <si>
+    <t>a9_b37_18</t>
+  </si>
+  <si>
+    <t>a9_b40_18</t>
+  </si>
+  <si>
+    <t>a9_b43_18</t>
+  </si>
+  <si>
+    <t>a9_w2_18</t>
+  </si>
+  <si>
+    <t>a9_w4_18</t>
+  </si>
+  <si>
+    <t>a24_w6_18</t>
+  </si>
+  <si>
+    <t>a9_w10_18</t>
+  </si>
+  <si>
+    <t>a9_w11_18</t>
+  </si>
+  <si>
+    <t>a9_w13_18</t>
+  </si>
+  <si>
+    <t>a9_w15_18</t>
+  </si>
+  <si>
+    <t>a9_w20_18</t>
+  </si>
+  <si>
+    <t>a9_w28_18</t>
+  </si>
+  <si>
+    <t>a9_w30_18</t>
+  </si>
+  <si>
+    <t>a9_w34_18</t>
+  </si>
+  <si>
+    <t>Genetic control samples; cohorts 7+22 (2018-09-06); cohort day 8+23 (2018-09-07); cohort day 9 + 24 2018-09-08 ( respirometry day 15)</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +2022,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1993,6 +2068,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2055,7 +2136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2090,13 +2171,16 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2826,19 +2910,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3219,19 +3303,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3638,19 +3722,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4084,19 +4168,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4110,8 +4194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6D1863-FB1E-4A2C-8DF3-AD7479E9B178}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4133,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>622</v>
+        <v>648</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4157,7 +4241,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4203,31 +4287,31 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>586</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="14" t="s">
         <v>589</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="14" t="s">
         <v>590</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="14" t="s">
         <v>591</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="14" t="s">
         <v>592</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="14" t="s">
         <v>593</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="14" t="s">
         <v>594</v>
       </c>
       <c r="L9" s="13"/>
@@ -4236,31 +4320,31 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>597</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="14" t="s">
         <v>598</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>599</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="14" t="s">
         <v>600</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="14" t="s">
         <v>601</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="14" t="s">
         <v>602</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="14" t="s">
         <v>603</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="14" t="s">
         <v>605</v>
       </c>
       <c r="L10" s="13"/>
@@ -4269,32 +4353,32 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>596</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>609</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>610</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="H11" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>613</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>614</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>615</v>
       </c>
       <c r="L11" s="13"/>
     </row>
@@ -4303,73 +4387,125 @@
         <v>4</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>618</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>608</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>607</v>
-      </c>
-      <c r="H12" s="9" t="s">
+      <c r="I12" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="K12" s="13"/>
+      <c r="K12" s="17" t="s">
+        <v>623</v>
+      </c>
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="C13" s="17" t="s">
+        <v>624</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>626</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>628</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>629</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>630</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>632</v>
+      </c>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="C14" s="17" t="s">
+        <v>633</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>637</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>639</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>641</v>
+      </c>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
+      <c r="C15" s="17" t="s">
+        <v>642</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>644</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>647</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>647</v>
+      </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -4420,19 +4556,19 @@
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4673,19 +4809,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4974,19 +5110,19 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5236,19 +5372,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5526,19 +5662,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5940,19 +6076,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6334,19 +6470,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6724,19 +6860,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update data and freezer boxes
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03A276B-9B2F-4974-A0F2-5F3B7B090DF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F07ECC5-82AA-4D77-8AC2-DAE38B6DED9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="5" activeTab="14" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="5" activeTab="16" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="813">
   <si>
     <t>Date</t>
   </si>
@@ -2295,12 +2295,6 @@
     <t>A2-13-5</t>
   </si>
   <si>
-    <t xml:space="preserve"> cohort 2018-09-11(day 12+27) [1 sample]; 2018-09-12 cohort (day 13) </t>
-  </si>
-  <si>
-    <t>NB#005, pg 24,25</t>
-  </si>
-  <si>
     <t>A2-13-6</t>
   </si>
   <si>
@@ -2341,6 +2335,156 @@
   </si>
   <si>
     <t>A7RT-G6</t>
+  </si>
+  <si>
+    <t>A2-14-1</t>
+  </si>
+  <si>
+    <t>A2-14-2</t>
+  </si>
+  <si>
+    <t>A2-14-3</t>
+  </si>
+  <si>
+    <t>A2-14-4</t>
+  </si>
+  <si>
+    <t>A2-14-5</t>
+  </si>
+  <si>
+    <t>A2-14-6</t>
+  </si>
+  <si>
+    <t>A2-14-7</t>
+  </si>
+  <si>
+    <t>A2-14-8</t>
+  </si>
+  <si>
+    <t>A2-14-9</t>
+  </si>
+  <si>
+    <t>A2-15-9</t>
+  </si>
+  <si>
+    <t>A2-14-10</t>
+  </si>
+  <si>
+    <t>A2-14-11</t>
+  </si>
+  <si>
+    <t>A2-14-12</t>
+  </si>
+  <si>
+    <t>A2-14-13</t>
+  </si>
+  <si>
+    <t>A2-14-14</t>
+  </si>
+  <si>
+    <t>A2-14-15</t>
+  </si>
+  <si>
+    <t>A2-14-16</t>
+  </si>
+  <si>
+    <t>A2-14-17</t>
+  </si>
+  <si>
+    <t>A2-14-18</t>
+  </si>
+  <si>
+    <t>A2-14-19</t>
+  </si>
+  <si>
+    <t>A2-14-20</t>
+  </si>
+  <si>
+    <t>A2-14-21</t>
+  </si>
+  <si>
+    <t>A2-14-22</t>
+  </si>
+  <si>
+    <t>A2-14-23</t>
+  </si>
+  <si>
+    <t>A2-14-24</t>
+  </si>
+  <si>
+    <t>A2-14-25</t>
+  </si>
+  <si>
+    <t>A2-14-26</t>
+  </si>
+  <si>
+    <t>A2-14-27</t>
+  </si>
+  <si>
+    <t>A2-14-28</t>
+  </si>
+  <si>
+    <t>A2-14-29</t>
+  </si>
+  <si>
+    <t>A2-14-30</t>
+  </si>
+  <si>
+    <t>A2-15-1</t>
+  </si>
+  <si>
+    <t>A2-15-2</t>
+  </si>
+  <si>
+    <t>A2-15-3</t>
+  </si>
+  <si>
+    <t>A2-15-4</t>
+  </si>
+  <si>
+    <t>A2-15-5</t>
+  </si>
+  <si>
+    <t>A2-15-6</t>
+  </si>
+  <si>
+    <t>A2-15-7</t>
+  </si>
+  <si>
+    <t>A2-15-8</t>
+  </si>
+  <si>
+    <t>A2-15-10</t>
+  </si>
+  <si>
+    <t>A2-15-11</t>
+  </si>
+  <si>
+    <t>A2-15-12</t>
+  </si>
+  <si>
+    <t>A2-15-13</t>
+  </si>
+  <si>
+    <t>A2-15-14</t>
+  </si>
+  <si>
+    <t>A2-15-15</t>
+  </si>
+  <si>
+    <t>A2-15-16</t>
+  </si>
+  <si>
+    <t>A2-15-17</t>
+  </si>
+  <si>
+    <t>A2-15-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cohort 2018-09-11(day 12+27) [1 sample]; 2018-09-12 cohort (day 13) ; 2018-09-13 cohor t(day 14); 2018-09-14 cohort (day 15)</t>
+  </si>
+  <si>
+    <t>NB#005, pg 24,25, 44</t>
   </si>
 </sst>
 </file>
@@ -4959,7 +5103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F41B0-8C96-400C-99C2-08CF3B9A4A24}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -5065,16 +5209,16 @@
         <v>740</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>759</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>760</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>761</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>762</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>763</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>764</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -5770,8 +5914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE7528C-92A9-4AA3-A9F6-E6E2787FAB31}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5793,7 +5937,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>749</v>
+        <v>811</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -5822,7 +5966,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>750</v>
+        <v>812</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5882,10 +6026,10 @@
         <v>748</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="3"/>
@@ -5895,28 +6039,28 @@
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>751</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>752</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>753</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>754</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>755</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>756</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>757</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="J10" s="14" t="s">
         <v>758</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>759</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>760</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="3"/>
@@ -5925,14 +6069,30 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="C11" s="13" t="s">
+        <v>763</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>764</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>765</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>766</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>767</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>768</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>769</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>770</v>
+      </c>
       <c r="K11" s="13"/>
       <c r="L11" s="3"/>
     </row>
@@ -5940,28 +6100,60 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="C12" s="13" t="s">
+        <v>771</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>773</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>774</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>775</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>776</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>777</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>778</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>779</v>
+      </c>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="C13" s="13" t="s">
+        <v>780</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>781</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>782</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>783</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>784</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>785</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>786</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>787</v>
+      </c>
       <c r="K13" s="13"/>
       <c r="L13" s="3"/>
     </row>
@@ -5969,14 +6161,30 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="C14" s="13" t="s">
+        <v>788</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>789</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>790</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>791</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>792</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>793</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>794</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>795</v>
+      </c>
       <c r="K14" s="13"/>
       <c r="L14" s="3"/>
     </row>
@@ -5984,14 +6192,30 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="C15" s="13" t="s">
+        <v>796</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>797</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>798</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>799</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>800</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>801</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>772</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>802</v>
+      </c>
       <c r="K15" s="13"/>
       <c r="L15" s="3"/>
     </row>
@@ -5999,14 +6223,30 @@
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="C16" s="13" t="s">
+        <v>803</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>804</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>805</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>806</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>807</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>808</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>809</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>810</v>
+      </c>
       <c r="K16" s="13"/>
       <c r="L16" s="3"/>
     </row>
@@ -6056,12 +6296,7 @@
       <c r="L19" s="18"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>732</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>733</v>
-      </c>
+      <c r="B21"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D26"/>

</xml_diff>

<commit_message>
updating storage and dataset
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4654BF9-88A2-4B0D-AE66-8B6CA96FCA13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571EC3DB-145F-4B8B-8AE4-B1D66059AD26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="5" activeTab="14" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="5" activeTab="17" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="924">
   <si>
     <t>Date</t>
   </si>
@@ -2635,12 +2635,6 @@
     <t>A2-17-30</t>
   </si>
   <si>
-    <t>cohort 2018-09-15, day 16; cohort 2018-09-16, day 17</t>
-  </si>
-  <si>
-    <t>NB#005, pg 49, 51</t>
-  </si>
-  <si>
     <t>A13RT-E10</t>
   </si>
   <si>
@@ -2690,6 +2684,141 @@
   </si>
   <si>
     <t>h11w28_18</t>
+  </si>
+  <si>
+    <t>A2-19-1</t>
+  </si>
+  <si>
+    <t>A2-19-2</t>
+  </si>
+  <si>
+    <t>A2-19-3</t>
+  </si>
+  <si>
+    <t>A2-19-4</t>
+  </si>
+  <si>
+    <t>A2-19-5</t>
+  </si>
+  <si>
+    <t>A2-19-6</t>
+  </si>
+  <si>
+    <t>A2-19-7</t>
+  </si>
+  <si>
+    <t>A2-19-8</t>
+  </si>
+  <si>
+    <t>A2-19-9</t>
+  </si>
+  <si>
+    <t>A2-19-10</t>
+  </si>
+  <si>
+    <t>A2-19-11</t>
+  </si>
+  <si>
+    <t>A2-19-12</t>
+  </si>
+  <si>
+    <t>A2-19-13</t>
+  </si>
+  <si>
+    <t>A2-19-14</t>
+  </si>
+  <si>
+    <t>A2-19-15</t>
+  </si>
+  <si>
+    <t>A2-19-16</t>
+  </si>
+  <si>
+    <t>A2-19-17</t>
+  </si>
+  <si>
+    <t>A2-19-18</t>
+  </si>
+  <si>
+    <t>A2-18-1</t>
+  </si>
+  <si>
+    <t>A2-18-2</t>
+  </si>
+  <si>
+    <t>A2-18-3</t>
+  </si>
+  <si>
+    <t>A2-18-4</t>
+  </si>
+  <si>
+    <t>A2-18-5</t>
+  </si>
+  <si>
+    <t>A2-18-6</t>
+  </si>
+  <si>
+    <t>A2-18-7</t>
+  </si>
+  <si>
+    <t>A2-18-8</t>
+  </si>
+  <si>
+    <t>A2-18-9</t>
+  </si>
+  <si>
+    <t>A2-18-10</t>
+  </si>
+  <si>
+    <t>A2-18-11</t>
+  </si>
+  <si>
+    <t>A2-18-12</t>
+  </si>
+  <si>
+    <t>A2-18-13</t>
+  </si>
+  <si>
+    <t>A2-18-14</t>
+  </si>
+  <si>
+    <t>A2-18-15</t>
+  </si>
+  <si>
+    <t>A2-18-16</t>
+  </si>
+  <si>
+    <t>A2-18-17</t>
+  </si>
+  <si>
+    <t>A2-18-18</t>
+  </si>
+  <si>
+    <t>A2-18-19</t>
+  </si>
+  <si>
+    <t>A2-18-20</t>
+  </si>
+  <si>
+    <t>A2-18-21</t>
+  </si>
+  <si>
+    <t>A2-18-22</t>
+  </si>
+  <si>
+    <t>A2-18-23</t>
+  </si>
+  <si>
+    <t>A2-18-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cohort 2018-09-15, day 16; cohort 2018-09-16, day 17; 2018-09-17 day 18 cohort; 2018-09-18 day 19 cohort </t>
+  </si>
+  <si>
+    <t>NB#005, pg 49, 51, 62, 59</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -2727,7 +2856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2794,6 +2923,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -2853,7 +2994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2904,6 +3045,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5308,7 +5455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F41B0-8C96-400C-99C2-08CF3B9A4A24}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -5440,34 +5587,34 @@
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>862</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>868</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>867</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>863</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>865</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>878</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>869</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>870</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>866</v>
+      </c>
+      <c r="L10" s="13" t="s">
         <v>864</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>870</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>869</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>865</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>867</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>880</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>871</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>872</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>868</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5475,25 +5622,25 @@
         <v>3</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>871</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>874</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>873</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="F11" s="9" t="s">
+        <v>872</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>876</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>875</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>874</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="I11" s="9" t="s">
         <v>877</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>878</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>879</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -6627,8 +6774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44F610C-BDB4-48D0-9BB5-34A358C2AC95}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6650,7 +6797,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>862</v>
+        <v>921</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -6666,7 +6813,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>741</v>
+        <v>923</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -6679,7 +6826,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>863</v>
+        <v>922</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6720,31 +6867,31 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="20" t="s">
         <v>817</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="20" t="s">
         <v>818</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="20" t="s">
         <v>819</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="20" t="s">
         <v>820</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="20" t="s">
         <v>821</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="20" t="s">
         <v>822</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="20" t="s">
         <v>823</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="20" t="s">
         <v>824</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="20" t="s">
         <v>825</v>
       </c>
       <c r="L9" s="3"/>
@@ -6753,58 +6900,58 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="20" t="s">
         <v>826</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="20" t="s">
         <v>827</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="20" t="s">
         <v>828</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="20" t="s">
         <v>829</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="20" t="s">
         <v>830</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="20" t="s">
         <v>831</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="21" t="s">
         <v>832</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="21" t="s">
         <v>833</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="21" t="s">
         <v>834</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="21" t="s">
         <v>835</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="21" t="s">
         <v>836</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="21" t="s">
         <v>837</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="21" t="s">
         <v>838</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="21" t="s">
         <v>839</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="21" t="s">
         <v>840</v>
       </c>
       <c r="L11" s="3"/>
@@ -6813,31 +6960,31 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="21" t="s">
         <v>841</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="21" t="s">
         <v>842</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="21" t="s">
         <v>843</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="21" t="s">
         <v>844</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="21" t="s">
         <v>845</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="21" t="s">
         <v>846</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="21" t="s">
         <v>847</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="21" t="s">
         <v>848</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="21" t="s">
         <v>849</v>
       </c>
     </row>
@@ -6845,31 +6992,31 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="21" t="s">
         <v>850</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="21" t="s">
         <v>851</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="21" t="s">
         <v>852</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="21" t="s">
         <v>853</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="21" t="s">
         <v>854</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="21" t="s">
         <v>855</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="21" t="s">
         <v>856</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="21" t="s">
         <v>857</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="21" t="s">
         <v>858</v>
       </c>
       <c r="L13" s="3"/>
@@ -6878,81 +7025,165 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="21" t="s">
         <v>859</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="21" t="s">
         <v>860</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="21" t="s">
         <v>861</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="F14" s="17" t="s">
+        <v>897</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>898</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>899</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>900</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>901</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>902</v>
+      </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="C15" s="17" t="s">
+        <v>903</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>904</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>905</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>906</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>907</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>908</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>909</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>910</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>911</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="C16" s="17" t="s">
+        <v>912</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>913</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>914</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>915</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>916</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>917</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>918</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>919</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>920</v>
+      </c>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="C17" s="12" t="s">
+        <v>879</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>880</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>881</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>882</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>883</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>884</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>885</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>886</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>887</v>
+      </c>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
+      <c r="C18" s="12" t="s">
+        <v>888</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>889</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>890</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>891</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>892</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>893</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>894</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>895</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>896</v>
+      </c>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
adding weight data and updating storage box info
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571EC3DB-145F-4B8B-8AE4-B1D66059AD26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2833CE56-3717-404A-A57A-28FBE14C44F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="5" activeTab="17" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="6" activeTab="14" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="R4P8" sheetId="23" r:id="rId16"/>
     <sheet name="R4_P9" sheetId="24" r:id="rId17"/>
     <sheet name="R4_P10" sheetId="25" r:id="rId18"/>
+    <sheet name="R4_P11" sheetId="26" r:id="rId19"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="937">
   <si>
     <t>Date</t>
   </si>
@@ -2819,6 +2820,45 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>2018-00-04 started</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>A2-20-1</t>
+  </si>
+  <si>
+    <t>A2-20-2</t>
+  </si>
+  <si>
+    <t>A2-20-3</t>
+  </si>
+  <si>
+    <t>A2-20-4</t>
+  </si>
+  <si>
+    <t>A2-20-5</t>
+  </si>
+  <si>
+    <t>A2-20-6</t>
+  </si>
+  <si>
+    <t>A2-20-7</t>
+  </si>
+  <si>
+    <t>cohort 2018-09-19 apple, day 20</t>
+  </si>
+  <si>
+    <t>All apple cohorts</t>
+  </si>
+  <si>
+    <t>all apple cohorts</t>
+  </si>
+  <si>
+    <t>genetic controls for 2018 pupal collection; cohorts 2018-09-09 (day 10+25); cohort 2018-09-10(day 11+26); cohort 2018-09-11(day 12+27) ; all apple cohorts</t>
   </si>
 </sst>
 </file>
@@ -3041,16 +3081,16 @@
     <xf numFmtId="49" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3780,19 +3820,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4173,19 +4213,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4592,19 +4632,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5038,19 +5078,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5429,19 +5469,19 @@
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5455,8 +5495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F41B0-8C96-400C-99C2-08CF3B9A4A24}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5551,31 +5591,31 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>738</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>739</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>740</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>759</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>760</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>761</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>762</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>813</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>814</v>
       </c>
       <c r="L9" s="13" t="s">
@@ -5586,31 +5626,31 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>862</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>868</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>867</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>863</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>865</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>878</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>869</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>870</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>866</v>
       </c>
       <c r="L10" s="13" t="s">
@@ -5621,87 +5661,87 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>871</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>874</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="13" t="s">
         <v>873</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="13" t="s">
         <v>872</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="13" t="s">
         <v>876</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="13" t="s">
         <v>877</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="15"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
@@ -5752,19 +5792,19 @@
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5778,8 +5818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAB82DF-5EF5-434D-96B2-341D5EC857C2}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5825,7 +5865,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>708</v>
+        <v>936</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -6200,19 +6240,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -6307,7 +6347,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6352,6 +6392,9 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -6673,19 +6716,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
@@ -6774,8 +6817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44F610C-BDB4-48D0-9BB5-34A358C2AC95}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6820,6 +6863,9 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -6867,31 +6913,31 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>817</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>818</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>819</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="18" t="s">
         <v>820</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="18" t="s">
         <v>821</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="18" t="s">
         <v>822</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="18" t="s">
         <v>823</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="18" t="s">
         <v>824</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="K9" s="18" t="s">
         <v>825</v>
       </c>
       <c r="L9" s="3"/>
@@ -6900,58 +6946,58 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>826</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="18" t="s">
         <v>827</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="18" t="s">
         <v>828</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="18" t="s">
         <v>829</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="18" t="s">
         <v>830</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="18" t="s">
         <v>831</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>832</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>833</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>834</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="19" t="s">
         <v>835</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="19" t="s">
         <v>836</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="19" t="s">
         <v>837</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>838</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="19" t="s">
         <v>839</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="19" t="s">
         <v>840</v>
       </c>
       <c r="L11" s="3"/>
@@ -6960,31 +7006,31 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>841</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>842</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>843</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>844</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="19" t="s">
         <v>845</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="19" t="s">
         <v>846</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="19" t="s">
         <v>847</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="19" t="s">
         <v>848</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="19" t="s">
         <v>849</v>
       </c>
     </row>
@@ -6992,31 +7038,31 @@
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>850</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>851</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>852</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="19" t="s">
         <v>853</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>854</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="19" t="s">
         <v>855</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="19" t="s">
         <v>856</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="19" t="s">
         <v>857</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="19" t="s">
         <v>858</v>
       </c>
       <c r="L13" s="3"/>
@@ -7025,13 +7071,13 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>859</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>860</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="19" t="s">
         <v>861</v>
       </c>
       <c r="F14" s="17" t="s">
@@ -7187,19 +7233,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
@@ -7274,6 +7320,357 @@
       <c r="D48"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B19:L19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03B48B6-7D7C-46A3-A16E-73A037A5E80A}">
+  <dimension ref="A1:L49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>926</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>927</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>928</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>929</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>930</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>931</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>932</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+    </row>
+    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21"/>
+    </row>
+    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D49"/>
     </row>
   </sheetData>
@@ -7515,19 +7912,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7816,19 +8213,19 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8078,19 +8475,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8368,19 +8765,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8782,19 +9179,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9176,19 +9573,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9566,19 +9963,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updating data storage information
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D8FF4E-FDE5-4A02-BAFE-7D14C8B47B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C7164B-F565-4DC9-9712-818E78DD5879}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="6" activeTab="14" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="7" activeTab="19" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="R4_P9" sheetId="24" r:id="rId17"/>
     <sheet name="R4_P10" sheetId="25" r:id="rId18"/>
     <sheet name="R4_P11" sheetId="26" r:id="rId19"/>
+    <sheet name="Sheet2" sheetId="27" r:id="rId20"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="1072">
   <si>
     <t>Date</t>
   </si>
@@ -2849,9 +2850,6 @@
     <t>A2-20-7</t>
   </si>
   <si>
-    <t>cohort 2018-09-19 apple, day 20</t>
-  </si>
-  <si>
     <t>All apple cohorts</t>
   </si>
   <si>
@@ -3003,6 +3001,270 @@
   </si>
   <si>
     <t>A2RT-1</t>
+  </si>
+  <si>
+    <t>h3b3_18</t>
+  </si>
+  <si>
+    <t>h3b5_18</t>
+  </si>
+  <si>
+    <t>h3b15_18</t>
+  </si>
+  <si>
+    <t>h3b25_18</t>
+  </si>
+  <si>
+    <t>h3b26_18</t>
+  </si>
+  <si>
+    <t>h3b27_18</t>
+  </si>
+  <si>
+    <t>h3b33_18</t>
+  </si>
+  <si>
+    <t>h3b35_18</t>
+  </si>
+  <si>
+    <t>h3b36_18</t>
+  </si>
+  <si>
+    <t>h3b39_18</t>
+  </si>
+  <si>
+    <t>h3b44_18</t>
+  </si>
+  <si>
+    <t>h3b45_18</t>
+  </si>
+  <si>
+    <t>h3w2_18</t>
+  </si>
+  <si>
+    <t>h3w7_18</t>
+  </si>
+  <si>
+    <t>h3w8_18</t>
+  </si>
+  <si>
+    <t>h3w11_18</t>
+  </si>
+  <si>
+    <t>h3w12_18</t>
+  </si>
+  <si>
+    <t>h3w22_18</t>
+  </si>
+  <si>
+    <t>h3w29_18</t>
+  </si>
+  <si>
+    <t>h3w33_18</t>
+  </si>
+  <si>
+    <t>h3w34_18</t>
+  </si>
+  <si>
+    <t>h3w35_18</t>
+  </si>
+  <si>
+    <t>h3w44_18</t>
+  </si>
+  <si>
+    <t>h3w45_18</t>
+  </si>
+  <si>
+    <t>A3-3-1</t>
+  </si>
+  <si>
+    <t>A2-24-1</t>
+  </si>
+  <si>
+    <t>A2-24-2</t>
+  </si>
+  <si>
+    <t>A2-24-3</t>
+  </si>
+  <si>
+    <t>NB#005, pg 66, 81 , 87, 73, 85</t>
+  </si>
+  <si>
+    <t>cohort 2018-09-19 apple, day 20; cohort 2018-09-22, day 2 HAW; cohort 2018-09-20,day21, APPLE; cohort 2018-09-23, day 3, HAW ; cohort day 3+24, 2018-09-24, APPLE</t>
+  </si>
+  <si>
+    <t>2018-10-09</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>NB#005, pg 92, 96</t>
+  </si>
+  <si>
+    <t>cohort day 4 , 2018-09-24, HAWTHORN; cohort day 5, 2018-09-25, HAWTHORN</t>
+  </si>
+  <si>
+    <t>h4o4_18</t>
+  </si>
+  <si>
+    <t>h4o6_18</t>
+  </si>
+  <si>
+    <t>h4o7_18</t>
+  </si>
+  <si>
+    <t>h4o8_18</t>
+  </si>
+  <si>
+    <t>h4o9_18</t>
+  </si>
+  <si>
+    <t>h4o14_18</t>
+  </si>
+  <si>
+    <t>h4o16_18</t>
+  </si>
+  <si>
+    <t>h4o18_18</t>
+  </si>
+  <si>
+    <t>h4o21_18</t>
+  </si>
+  <si>
+    <t>h4o28_18</t>
+  </si>
+  <si>
+    <t>h4o29_18</t>
+  </si>
+  <si>
+    <t>h4o31_18</t>
+  </si>
+  <si>
+    <t>h4o39_18</t>
+  </si>
+  <si>
+    <t>h4o42_18</t>
+  </si>
+  <si>
+    <t>h4o44_18</t>
+  </si>
+  <si>
+    <t>h4r1_18</t>
+  </si>
+  <si>
+    <t>h4r4_18</t>
+  </si>
+  <si>
+    <t>h4r11_18</t>
+  </si>
+  <si>
+    <t>h4r14_18</t>
+  </si>
+  <si>
+    <t>h4r16_18</t>
+  </si>
+  <si>
+    <t>h4r26_18</t>
+  </si>
+  <si>
+    <t>h4r30_18</t>
+  </si>
+  <si>
+    <t>h4r31_18</t>
+  </si>
+  <si>
+    <t>h4r32_18</t>
+  </si>
+  <si>
+    <t>h4r35_18</t>
+  </si>
+  <si>
+    <t>h4r37_18</t>
+  </si>
+  <si>
+    <t>h4r42_18</t>
+  </si>
+  <si>
+    <t>h4r45_18</t>
+  </si>
+  <si>
+    <t>h5w1_18</t>
+  </si>
+  <si>
+    <t>h5w3_18</t>
+  </si>
+  <si>
+    <t>h5w5_18</t>
+  </si>
+  <si>
+    <t>h5w9_18</t>
+  </si>
+  <si>
+    <t>h5w10_18</t>
+  </si>
+  <si>
+    <t>h5w11_18</t>
+  </si>
+  <si>
+    <t>h5w13_18</t>
+  </si>
+  <si>
+    <t>h5w16_18</t>
+  </si>
+  <si>
+    <t>h5w20_18</t>
+  </si>
+  <si>
+    <t>h5w22_18</t>
+  </si>
+  <si>
+    <t>h5w26_18</t>
+  </si>
+  <si>
+    <t>h5w29_18</t>
+  </si>
+  <si>
+    <t>h5w31_18</t>
+  </si>
+  <si>
+    <t>h5w32_18</t>
+  </si>
+  <si>
+    <t>h5w36_18</t>
+  </si>
+  <si>
+    <t>h5w41_18</t>
+  </si>
+  <si>
+    <t>h5w42_18</t>
+  </si>
+  <si>
+    <t>h5b5_18</t>
+  </si>
+  <si>
+    <t>h5b9_18</t>
+  </si>
+  <si>
+    <t>h5b14_18</t>
+  </si>
+  <si>
+    <t>h5b19_18</t>
+  </si>
+  <si>
+    <t>h5b20_18</t>
+  </si>
+  <si>
+    <t>h5b27_18</t>
+  </si>
+  <si>
+    <t>h5b30_18</t>
+  </si>
+  <si>
+    <t>h5b32_18</t>
+  </si>
+  <si>
+    <t>h5b42_18</t>
   </si>
 </sst>
 </file>
@@ -5639,7 +5901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D78F41B0-8C96-400C-99C2-08CF3B9A4A24}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -5827,13 +6089,13 @@
         <v>877</v>
       </c>
       <c r="J11" s="13" t="s">
+        <v>936</v>
+      </c>
+      <c r="K11" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="K11" s="13" t="s">
-        <v>938</v>
-      </c>
       <c r="L11" s="13" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -5841,31 +6103,31 @@
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="H12" s="13" t="s">
+        <v>980</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>981</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>982</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>983</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>984</v>
       </c>
       <c r="L12" s="13"/>
     </row>
@@ -6033,7 +6295,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -6561,7 +6823,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -7032,7 +7294,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -7502,8 +7764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03B48B6-7D7C-46A3-A16E-73A037A5E80A}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -7525,7 +7787,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>933</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -7552,6 +7814,9 @@
     <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1012</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7614,10 +7879,10 @@
         <v>932</v>
       </c>
       <c r="J9" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="K9" s="13" t="s">
         <v>939</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>940</v>
       </c>
       <c r="L9" s="3"/>
     </row>
@@ -7626,31 +7891,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>940</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>942</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>943</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>944</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>945</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="I10" s="13" t="s">
         <v>946</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>947</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="K10" s="13" t="s">
         <v>948</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>949</v>
       </c>
       <c r="L10" s="3"/>
     </row>
@@ -7659,31 +7924,31 @@
         <v>3</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>949</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>950</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>951</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>952</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>953</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>954</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>955</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>956</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>957</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>958</v>
       </c>
       <c r="L11" s="3"/>
     </row>
@@ -7692,31 +7957,31 @@
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
+        <v>958</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>959</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>960</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>961</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>962</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>963</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="I12" s="13" t="s">
         <v>964</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>965</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>966</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -7724,72 +7989,128 @@
         <v>5</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>967</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>968</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="E13" s="13" t="s">
+        <v>973</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>969</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>974</v>
-      </c>
-      <c r="F13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>970</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>971</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>972</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>973</v>
-      </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
+      <c r="J13" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>985</v>
+      </c>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="C14" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>994</v>
+      </c>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="C15" s="2" t="s">
+        <v>995</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>996</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>1003</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="C16" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>1011</v>
+      </c>
       <c r="K16" s="13"/>
       <c r="L16" s="3"/>
     </row>
@@ -8172,6 +8493,532 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557B291E-D48D-410F-9190-2421762F671A}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>1024</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>1026</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>1043</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>1049</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>1051</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>1052</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>1058</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1066</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1067</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>1071</v>
+      </c>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+    </row>
+    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B47"/>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B48"/>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B49"/>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B19:L19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
day 5 cohort apple 3rd collection date
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C7164B-F565-4DC9-9712-818E78DD5879}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CED30D7-85E7-47AE-B079-ED7634CB4651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="7" activeTab="19" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="7" activeTab="18" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1076">
   <si>
     <t>Date</t>
   </si>
@@ -3087,12 +3087,6 @@
     <t>A2-24-3</t>
   </si>
   <si>
-    <t>NB#005, pg 66, 81 , 87, 73, 85</t>
-  </si>
-  <si>
-    <t>cohort 2018-09-19 apple, day 20; cohort 2018-09-22, day 2 HAW; cohort 2018-09-20,day21, APPLE; cohort 2018-09-23, day 3, HAW ; cohort day 3+24, 2018-09-24, APPLE</t>
-  </si>
-  <si>
     <t>2018-10-09</t>
   </si>
   <si>
@@ -3265,6 +3259,24 @@
   </si>
   <si>
     <t>h5b42_18</t>
+  </si>
+  <si>
+    <t>A3-5-1</t>
+  </si>
+  <si>
+    <t>A3-5-2</t>
+  </si>
+  <si>
+    <t>A3-5-3</t>
+  </si>
+  <si>
+    <t>A3-5-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cohort 2018-09-19 apple, day 20; cohort 2018-09-22, day 2 HAW; cohort 2018-09-20,day21, APPLE; cohort 2018-09-23, day 3, HAW ; cohort day 3+24, 2018-09-24, APPLE; cohort day 5 , 2018-09-25, APPLE </t>
+  </si>
+  <si>
+    <t>NB#005, pg 66, 81 , 87, 73, 85, 99</t>
   </si>
 </sst>
 </file>
@@ -7764,8 +7776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03B48B6-7D7C-46A3-A16E-73A037A5E80A}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -7787,7 +7799,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1013</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -7816,7 +7828,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1012</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8111,16 +8123,24 @@
       <c r="J16" s="13" t="s">
         <v>1011</v>
       </c>
-      <c r="K16" s="13"/>
+      <c r="K16" s="13" t="s">
+        <v>1070</v>
+      </c>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="C17" s="13" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>1073</v>
+      </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -8500,11 +8520,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557B291E-D48D-410F-9190-2421762F671A}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="15.375" style="2"/>
@@ -8515,7 +8535,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -8523,7 +8543,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -8539,7 +8559,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -8552,7 +8572,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8594,31 +8614,31 @@
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>1018</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>1021</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>1022</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>1023</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="K9" s="13" t="s">
         <v>1024</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>1025</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>1026</v>
       </c>
       <c r="L9" s="3"/>
     </row>
@@ -8627,31 +8647,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>1027</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>1028</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>1029</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>1030</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="I10" s="13" t="s">
         <v>1031</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>1032</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="K10" s="13" t="s">
         <v>1033</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>1034</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>1035</v>
       </c>
       <c r="L10" s="3"/>
     </row>
@@ -8660,31 +8680,31 @@
         <v>3</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>1036</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>1037</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>1038</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>1039</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>1040</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>1041</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>1042</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>1043</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>1044</v>
       </c>
       <c r="L11" s="3"/>
     </row>
@@ -8693,31 +8713,31 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>1046</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="I12" s="13" t="s">
         <v>1049</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>1050</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>1051</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>1052</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>1053</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -8725,31 +8745,31 @@
         <v>5</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>1054</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>1055</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>1056</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>1057</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>1058</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="J13" s="2" t="s">
         <v>1059</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="K13" s="2" t="s">
         <v>1060</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>1061</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>1062</v>
       </c>
       <c r="L13" s="3"/>
     </row>
@@ -8758,31 +8778,31 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>1063</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>1064</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>1065</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>1066</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>1067</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>1068</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>1069</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>1070</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>1071</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -8848,170 +8868,170 @@
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
     </row>
-    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>1046</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
         <v>1047</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>1049</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>1051</v>
       </c>
-      <c r="D26"/>
-    </row>
-    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>1052</v>
       </c>
-      <c r="D27"/>
-    </row>
-    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>1053</v>
       </c>
-      <c r="D28"/>
-    </row>
-    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>1054</v>
       </c>
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
         <v>1055</v>
       </c>
-      <c r="D30"/>
-    </row>
-    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>1056</v>
       </c>
-      <c r="D31"/>
-    </row>
-    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>1057</v>
       </c>
-      <c r="D32"/>
-    </row>
-    <row r="33" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>1058</v>
       </c>
-      <c r="D33"/>
-    </row>
-    <row r="34" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>1059</v>
       </c>
-      <c r="D34"/>
-    </row>
-    <row r="35" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>1060</v>
       </c>
-      <c r="D35"/>
-    </row>
-    <row r="36" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>1061</v>
       </c>
-      <c r="D36"/>
-    </row>
-    <row r="37" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>1062</v>
       </c>
-      <c r="D37"/>
-    </row>
-    <row r="38" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>1063</v>
       </c>
-      <c r="D38"/>
-    </row>
-    <row r="39" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>1064</v>
       </c>
-      <c r="D39"/>
-    </row>
-    <row r="40" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>1065</v>
       </c>
-      <c r="D40"/>
-    </row>
-    <row r="41" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>1066</v>
       </c>
-      <c r="D41"/>
-    </row>
-    <row r="42" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>1067</v>
       </c>
-      <c r="D42"/>
-    </row>
-    <row r="43" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>1068</v>
       </c>
-      <c r="D43"/>
-    </row>
-    <row r="44" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>1069</v>
       </c>
-      <c r="D44"/>
-    </row>
-    <row r="45" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>1070</v>
-      </c>
-      <c r="D45"/>
-    </row>
-    <row r="46" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>1071</v>
-      </c>
       <c r="D46"/>
     </row>
-    <row r="47" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new freezer position for tati, free run
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CED30D7-85E7-47AE-B079-ED7634CB4651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10927221-8C7D-46A7-8440-7B725682DFB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="7" activeTab="18" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="8" activeTab="20" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,8 @@
     <sheet name="R4_P9" sheetId="24" r:id="rId17"/>
     <sheet name="R4_P10" sheetId="25" r:id="rId18"/>
     <sheet name="R4_P11" sheetId="26" r:id="rId19"/>
-    <sheet name="Sheet2" sheetId="27" r:id="rId20"/>
+    <sheet name="R4_P12" sheetId="27" r:id="rId20"/>
+    <sheet name="R4_P13" sheetId="28" r:id="rId21"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="1076">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="1079">
   <si>
     <t>Date</t>
   </si>
@@ -3277,6 +3278,15 @@
   </si>
   <si>
     <t>NB#005, pg 66, 81 , 87, 73, 85, 99</t>
+  </si>
+  <si>
+    <t>2018-10-12</t>
+  </si>
+  <si>
+    <t>NB#005, 105</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -3452,7 +3462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3511,6 +3521,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7776,8 +7787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03B48B6-7D7C-46A3-A16E-73A037A5E80A}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -8520,8 +8531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557B291E-D48D-410F-9190-2421762F671A}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -9033,6 +9044,341 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B19:L19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17A8BC-CF1F-4D52-84AB-ABF99C09C81E}">
+  <dimension ref="A1:L49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9</v>
+      </c>
+      <c r="L8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+    </row>
+    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21"/>
+    </row>
+    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D49"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updating data sheet, storage box, and randomoization
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10927221-8C7D-46A7-8440-7B725682DFB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C6403-CC7E-4ABC-A48B-266765E47297}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="8" activeTab="20" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="10" activeTab="19" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="1093">
   <si>
     <t>Date</t>
   </si>
@@ -3094,12 +3094,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>NB#005, pg 92, 96</t>
-  </si>
-  <si>
-    <t>cohort day 4 , 2018-09-24, HAWTHORN; cohort day 5, 2018-09-25, HAWTHORN</t>
-  </si>
-  <si>
     <t>h4o4_18</t>
   </si>
   <si>
@@ -3287,6 +3281,54 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>A3-7-1</t>
+  </si>
+  <si>
+    <t>A3-7-2</t>
+  </si>
+  <si>
+    <t>A3-7-3</t>
+  </si>
+  <si>
+    <t>H-7-1</t>
+  </si>
+  <si>
+    <t>H-7-2</t>
+  </si>
+  <si>
+    <t>H-7-3</t>
+  </si>
+  <si>
+    <t>H-7-4</t>
+  </si>
+  <si>
+    <t>H-7-5</t>
+  </si>
+  <si>
+    <t>H-7-6</t>
+  </si>
+  <si>
+    <t>H-7-7</t>
+  </si>
+  <si>
+    <t>A3-7-4</t>
+  </si>
+  <si>
+    <t>H-7-8</t>
+  </si>
+  <si>
+    <t>H-7-9</t>
+  </si>
+  <si>
+    <t>H-7-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB#005, pg 92, 96, 108, </t>
+  </si>
+  <si>
+    <t>cohort day 4 , 2018-09-24, HAWTHORN; cohort day 5, 2018-09-25, HAWTHORN; cohort day 7, 2018-09-27, HAW + Apple</t>
   </si>
 </sst>
 </file>
@@ -3462,7 +3504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3515,13 +3557,17 @@
     <xf numFmtId="49" fontId="2" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4249,19 +4295,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4642,19 +4688,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5061,19 +5107,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5507,19 +5553,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5898,19 +5944,19 @@
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6245,19 +6291,19 @@
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6693,19 +6739,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -7169,19 +7215,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
@@ -7686,19 +7732,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
@@ -7810,7 +7856,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -7839,7 +7885,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8135,7 +8181,7 @@
         <v>1011</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="L16" s="3"/>
     </row>
@@ -8144,13 +8190,13 @@
         <v>9</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>1071</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>1072</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>1073</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -8176,19 +8222,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
@@ -8504,19 +8550,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8531,8 +8577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557B291E-D48D-410F-9190-2421762F671A}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -8554,7 +8600,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1015</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -8583,7 +8629,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1014</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8625,31 +8671,31 @@
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>1016</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>1017</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>1018</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>1019</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>1020</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>1021</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="K9" s="13" t="s">
         <v>1022</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>1023</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>1024</v>
       </c>
       <c r="L9" s="3"/>
     </row>
@@ -8658,31 +8704,31 @@
         <v>2</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>1025</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>1026</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>1027</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="H10" s="13" t="s">
         <v>1028</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="I10" s="13" t="s">
         <v>1029</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="J10" s="13" t="s">
         <v>1030</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="K10" s="13" t="s">
         <v>1031</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>1032</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>1033</v>
       </c>
       <c r="L10" s="3"/>
     </row>
@@ -8691,31 +8737,31 @@
         <v>3</v>
       </c>
       <c r="C11" s="13" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>1034</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>1035</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>1036</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>1037</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>1038</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>1039</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="K11" s="13" t="s">
         <v>1040</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>1041</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>1042</v>
       </c>
       <c r="L11" s="3"/>
     </row>
@@ -8723,32 +8769,32 @@
       <c r="B12" s="3">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="23" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>1043</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>1044</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="G12" s="13" t="s">
         <v>1045</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>1046</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="I12" s="13" t="s">
         <v>1047</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>1048</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>1049</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>1050</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -8756,31 +8802,31 @@
         <v>5</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>1052</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="F13" s="13" t="s">
         <v>1053</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>1054</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>1055</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>1056</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="J13" s="20" t="s">
         <v>1057</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="K13" s="20" t="s">
         <v>1058</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>1059</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>1060</v>
       </c>
       <c r="L13" s="3"/>
     </row>
@@ -8788,32 +8834,32 @@
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="24" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E14" s="24" t="s">
         <v>1061</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="24" t="s">
         <v>1062</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="24" t="s">
         <v>1063</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="24" t="s">
         <v>1064</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="I14" s="24" t="s">
         <v>1065</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="24" t="s">
         <v>1066</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="K14" s="24" t="s">
         <v>1067</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>1068</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>1069</v>
       </c>
       <c r="L14" s="3"/>
     </row>
@@ -8821,13 +8867,54 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
+      <c r="C15" s="24" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>1079</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>1081</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>1083</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>1084</v>
+      </c>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="C16" s="24" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>1090</v>
+      </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
@@ -8865,168 +8952,168 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D26"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D27"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D28"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="D29"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D30"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="D31"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D32"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="D33"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D34"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="D35"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D36"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D37"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D38"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D39"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D40"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="D41"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D42"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="D43"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D44"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D45"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D46"/>
     </row>
@@ -9057,11 +9144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17A8BC-CF1F-4D52-84AB-ABF99C09C81E}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="15.375" style="2"/>
@@ -9072,7 +9159,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -9090,7 +9177,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -9103,7 +9190,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9198,7 +9285,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="22"/>
+      <c r="L12" s="20"/>
     </row>
     <row r="13" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
@@ -9211,48 +9298,48 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
@@ -9291,93 +9378,93 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-    </row>
-    <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
-    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D26"/>
     </row>
-    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D27"/>
     </row>
-    <row r="28" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D28"/>
     </row>
-    <row r="29" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D29"/>
     </row>
-    <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D30"/>
     </row>
-    <row r="31" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D31"/>
     </row>
-    <row r="32" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D32"/>
     </row>
-    <row r="33" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33"/>
     </row>
-    <row r="34" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34"/>
     </row>
-    <row r="35" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35"/>
     </row>
-    <row r="36" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36"/>
     </row>
-    <row r="37" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37"/>
     </row>
-    <row r="38" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38"/>
     </row>
-    <row r="39" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39"/>
     </row>
-    <row r="40" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40"/>
     </row>
-    <row r="41" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41"/>
     </row>
-    <row r="42" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42"/>
     </row>
-    <row r="43" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43"/>
     </row>
-    <row r="44" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44"/>
     </row>
-    <row r="45" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45"/>
     </row>
-    <row r="46" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46"/>
     </row>
-    <row r="47" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47"/>
     </row>
-    <row r="48" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48"/>
     </row>
-    <row r="49" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49"/>
     </row>
   </sheetData>
@@ -9666,19 +9753,19 @@
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9928,19 +10015,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10218,19 +10305,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10632,19 +10719,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11026,19 +11113,19 @@
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11416,19 +11503,19 @@
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="2:12" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adding in data for collection 3 apple (2018-09-16) cohort 12 , 2018-10-02 cohort dat
</commit_message>
<xml_diff>
--- a/Data/Storage/2018_storage_minus80_information.xlsx
+++ b/Data/Storage/2018_storage_minus80_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatianagerena\Documents\GitHub\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew.nguyen\Desktop\Circadian_rhythm_runs_seasonal_timing\Data\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A109B-FC46-45F7-8A1D-35851A7F1E41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4F71A8-BBE3-4271-B462-47C17F8162B7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="9" activeTab="20" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
+    <workbookView xWindow="8715" yWindow="465" windowWidth="38235" windowHeight="23325" firstSheet="10" activeTab="22" xr2:uid="{11D8066D-8F91-E240-B83C-274814A92F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="R4_P12" sheetId="27" r:id="rId20"/>
     <sheet name="R4_P13" sheetId="28" r:id="rId21"/>
     <sheet name="RC_P9" sheetId="29" r:id="rId22"/>
+    <sheet name="RC_P10" sheetId="30" r:id="rId23"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1236">
   <si>
     <t>Date</t>
   </si>
@@ -3627,6 +3628,138 @@
   </si>
   <si>
     <t>a12r12_18</t>
+  </si>
+  <si>
+    <t>2018-10-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cohort day 9 (2018-09-29) apple + haw cohort; cohort day 10 (2018-09-30) apple + haw host; cohort day 11 (2018-10-01) apple + haw; cohort day 12 ( 2018-10-02) apple + haw </t>
+  </si>
+  <si>
+    <t>nb#005, pg 125, 129 , 114, 119</t>
+  </si>
+  <si>
+    <t>Chao's rack</t>
+  </si>
+  <si>
+    <t>H-9-1</t>
+  </si>
+  <si>
+    <t>H-9-2</t>
+  </si>
+  <si>
+    <t>H-9-3</t>
+  </si>
+  <si>
+    <t>H-9-4</t>
+  </si>
+  <si>
+    <t>H-9-5</t>
+  </si>
+  <si>
+    <t>H-9-6</t>
+  </si>
+  <si>
+    <t>H-9-7</t>
+  </si>
+  <si>
+    <t>H-9-8</t>
+  </si>
+  <si>
+    <t>H-9-9</t>
+  </si>
+  <si>
+    <t>H-9-10</t>
+  </si>
+  <si>
+    <t>H-10-1</t>
+  </si>
+  <si>
+    <t>H-10-2</t>
+  </si>
+  <si>
+    <t>H-10-3</t>
+  </si>
+  <si>
+    <t>H-10-4</t>
+  </si>
+  <si>
+    <t>H-10-5</t>
+  </si>
+  <si>
+    <t>H-10-6</t>
+  </si>
+  <si>
+    <t>H-10-7</t>
+  </si>
+  <si>
+    <t>H-10-8</t>
+  </si>
+  <si>
+    <t>H-10-9</t>
+  </si>
+  <si>
+    <t>H-10-10</t>
+  </si>
+  <si>
+    <t>A3-10-1</t>
+  </si>
+  <si>
+    <t>A3-10-2</t>
+  </si>
+  <si>
+    <t>A3-10-3</t>
+  </si>
+  <si>
+    <t>A3-10-4</t>
+  </si>
+  <si>
+    <t>H-11-1</t>
+  </si>
+  <si>
+    <t>H-11-2</t>
+  </si>
+  <si>
+    <t>H-11-3</t>
+  </si>
+  <si>
+    <t>H-11-4</t>
+  </si>
+  <si>
+    <t>H-11-5</t>
+  </si>
+  <si>
+    <t>A3-11-1</t>
+  </si>
+  <si>
+    <t>A3-11-2</t>
+  </si>
+  <si>
+    <t>A3-11-3</t>
+  </si>
+  <si>
+    <t>A3-12-1</t>
+  </si>
+  <si>
+    <t>A3-12-2</t>
+  </si>
+  <si>
+    <t>A3-12-3</t>
+  </si>
+  <si>
+    <t>A3-12-4</t>
+  </si>
+  <si>
+    <t>H-12-1</t>
+  </si>
+  <si>
+    <t>H-12-2</t>
+  </si>
+  <si>
+    <t>H-12-3</t>
+  </si>
+  <si>
+    <t>H-12-4</t>
   </si>
 </sst>
 </file>
@@ -9004,7 +9137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{557B291E-D48D-410F-9190-2421762F671A}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -9539,7 +9672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C17A8BC-CF1F-4D52-84AB-ABF99C09C81E}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -9895,8 +10028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9A39E7-9F01-4997-8771-0E6783C47772}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -10217,6 +10350,402 @@
       <c r="D47"/>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:K18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C741F9E5-90F2-482F-B373-24595820CBD9}">
+  <dimension ref="A1:K48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7</v>
+      </c>
+      <c r="J8" s="3">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>1200</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>1201</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>1202</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>1203</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>1210</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>1211</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>1212</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>3</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>1218</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>1219</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>1220</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>1221</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>1224</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>1225</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>1228</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>1230</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="2:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="2:11" ht="45.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="20" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20"/>
+    </row>
+    <row r="25" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="4:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D48"/>
     </row>
   </sheetData>

</xml_diff>